<commit_message>
spread email out by 1 second per email so it will email.  Updated initial file in of candidates to load new input.
</commit_message>
<xml_diff>
--- a/spec/fixtures/Invalid.xlsx
+++ b/spec/fixtures/Invalid.xlsx
@@ -13,9 +13,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
   <si>
-    <t>Year 2 Candidates attending The Way</t>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>1st name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grade </t>
+  </si>
+  <si>
+    <t>parents preferred email</t>
+  </si>
+  <si>
+    <t>Cardinal Gibbons HS Group</t>
   </si>
   <si>
     <t>Sophia</t>
@@ -33,16 +45,13 @@
     <t>joan3@nc.rr.com</t>
   </si>
   <si>
-    <t>Year 2 Candidates attending the Catholic HS teens sessions</t>
-  </si>
-  <si>
     <t>Annunziata</t>
   </si>
   <si>
     <t>Robert</t>
   </si>
   <si>
-    <t>@nc.rr.com; rannunz</t>
+    <t>@nc.rr.com, rannunz</t>
   </si>
   <si>
     <t>Bartos</t>
@@ -76,7 +85,6 @@
     </font>
     <font>
       <b val="1"/>
-      <i val="1"/>
       <u val="single"/>
       <sz val="11"/>
       <color indexed="8"/>
@@ -92,7 +100,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="9"/>
+        <fgColor indexed="10"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -107,16 +115,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="9"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="9"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="9"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="9"/>
       </bottom>
       <diagonal/>
     </border>
@@ -126,11 +134,14 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -139,10 +150,13 @@
     <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -168,8 +182,8 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1261,7 +1275,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1280,83 +1294,85 @@
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="B1" t="s" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="3">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" ht="15" customHeight="1">
       <c r="A2" s="5"/>
       <c r="B2" t="s" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s" s="5">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s" s="5">
-        <v>3</v>
-      </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
     </row>
     <row r="3" ht="15" customHeight="1">
       <c r="A3" t="s" s="5">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" t="s" s="5">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s" s="5">
-        <v>5</v>
-      </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
     </row>
     <row r="4" ht="15" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
     </row>
     <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="2">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="A5" t="s" s="5">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" t="s" s="5">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s" s="7">
+        <v>4</v>
+      </c>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" ht="15" customHeight="1">
       <c r="A6" t="s" s="5">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s" s="5">
-        <v>8</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" t="s" s="5">
-        <v>9</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" t="s" s="5">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" t="s" s="7">
+        <v>4</v>
+      </c>
+      <c r="F6" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1375,83 +1391,83 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="6" customWidth="1"/>
-    <col min="2" max="2" width="8.85156" style="6" customWidth="1"/>
-    <col min="3" max="3" width="8.85156" style="6" customWidth="1"/>
-    <col min="4" max="4" width="8.85156" style="6" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="6" customWidth="1"/>
-    <col min="6" max="256" width="8.85156" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.85156" style="8" customWidth="1"/>
+    <col min="2" max="2" width="8.85156" style="8" customWidth="1"/>
+    <col min="3" max="3" width="8.85156" style="8" customWidth="1"/>
+    <col min="4" max="4" width="8.85156" style="8" customWidth="1"/>
+    <col min="5" max="5" width="8.85156" style="8" customWidth="1"/>
+    <col min="6" max="256" width="8.85156" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" ht="15" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" ht="15" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" ht="15" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" ht="15" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" ht="15" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" ht="15" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" ht="15" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" ht="15" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" ht="15" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1470,83 +1486,83 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="7" customWidth="1"/>
-    <col min="2" max="2" width="8.85156" style="7" customWidth="1"/>
-    <col min="3" max="3" width="8.85156" style="7" customWidth="1"/>
-    <col min="4" max="4" width="8.85156" style="7" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="7" customWidth="1"/>
-    <col min="6" max="256" width="8.85156" style="7" customWidth="1"/>
+    <col min="1" max="1" width="8.85156" style="9" customWidth="1"/>
+    <col min="2" max="2" width="8.85156" style="9" customWidth="1"/>
+    <col min="3" max="3" width="8.85156" style="9" customWidth="1"/>
+    <col min="4" max="4" width="8.85156" style="9" customWidth="1"/>
+    <col min="5" max="5" width="8.85156" style="9" customWidth="1"/>
+    <col min="6" max="256" width="8.85156" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" ht="15" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" ht="15" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" ht="15" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" ht="15" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" ht="15" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" ht="15" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" ht="15" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" ht="15" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" ht="15" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added middle_name to candidate_sheet
</commit_message>
<xml_diff>
--- a/spec/fixtures/Invalid.xlsx
+++ b/spec/fixtures/Invalid.xlsx
@@ -1,19 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulkristoff/dev/confirmation/spec/fixtures/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="15960" windowHeight="16300"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Last Name</t>
   </si>
@@ -63,29 +79,16 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <u val="single"/>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -130,67 +133,103 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="001FB714"/>
+      <rgbColor rgb="000000D4"/>
+      <rgbColor rgb="00FCF305"/>
+      <rgbColor rgb="00F20884"/>
+      <rgbColor rgb="0000ABEA"/>
+      <rgbColor rgb="00900000"/>
+      <rgbColor rgb="00006411"/>
+      <rgbColor rgb="00000090"/>
+      <rgbColor rgb="0090713A"/>
+      <rgbColor rgb="004600A5"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -316,7 +355,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -325,7 +364,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -334,7 +373,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -408,7 +447,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -416,7 +455,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -435,7 +474,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -465,7 +504,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -491,7 +530,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -517,7 +556,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -543,7 +582,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -569,7 +608,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -595,7 +634,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -621,7 +660,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -647,7 +686,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -673,7 +712,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -686,9 +725,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -703,7 +748,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="38000"/>
             </a:srgbClr>
@@ -711,7 +756,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -730,7 +775,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -756,7 +801,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -782,7 +827,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -808,7 +853,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -834,7 +879,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -860,7 +905,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -886,7 +931,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -912,7 +957,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -938,7 +983,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -964,7 +1009,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -977,9 +1022,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -993,7 +1044,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1012,7 +1063,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1042,7 +1093,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1068,7 +1119,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1094,7 +1145,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1120,7 +1171,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1146,7 +1197,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1172,7 +1223,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1198,7 +1249,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1224,7 +1275,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1250,7 +1301,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1263,80 +1314,89 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85156" style="1" customWidth="1"/>
-    <col min="4" max="4" width="46.3516" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="46.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="18.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85156" style="1" customWidth="1"/>
-    <col min="7" max="256" width="8.85156" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="1" customWidth="1"/>
+    <col min="7" max="256" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="3">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" ht="15" customHeight="1">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
-      <c r="B2" t="s" s="5">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s" s="5">
+      <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s" s="5">
+      <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="5">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="5"/>
-      <c r="C3" t="s" s="5">
+      <c r="C3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s" s="5">
+      <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" ht="15" customHeight="1">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1344,39 +1404,39 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="5">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s" s="5">
+      <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="4"/>
-      <c r="D5" t="s" s="5">
+      <c r="D5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" t="s" s="7">
+      <c r="E5" s="7" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" t="s" s="5">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s" s="5">
+      <c r="B6" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="5"/>
-      <c r="E6" t="s" s="7">
+      <c r="E6" s="7" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -1384,85 +1444,81 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="8" customWidth="1"/>
-    <col min="2" max="2" width="8.85156" style="8" customWidth="1"/>
-    <col min="3" max="3" width="8.85156" style="8" customWidth="1"/>
-    <col min="4" max="4" width="8.85156" style="8" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="8" customWidth="1"/>
-    <col min="6" max="256" width="8.85156" style="8" customWidth="1"/>
+    <col min="1" max="5" width="8.83203125" style="8" customWidth="1"/>
+    <col min="6" max="256" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" ht="15" customHeight="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" ht="15" customHeight="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" ht="15" customHeight="1">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" ht="15" customHeight="1">
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" ht="15" customHeight="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1471,7 +1527,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -1479,85 +1535,81 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="9" customWidth="1"/>
-    <col min="2" max="2" width="8.85156" style="9" customWidth="1"/>
-    <col min="3" max="3" width="8.85156" style="9" customWidth="1"/>
-    <col min="4" max="4" width="8.85156" style="9" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="9" customWidth="1"/>
-    <col min="6" max="256" width="8.85156" style="9" customWidth="1"/>
+    <col min="1" max="5" width="8.83203125" style="9" customWidth="1"/>
+    <col min="6" max="256" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" ht="15" customHeight="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" ht="15" customHeight="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" ht="15" customHeight="1">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" ht="15" customHeight="1">
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" ht="15" customHeight="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1566,7 +1618,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
still getting tests working
</commit_message>
<xml_diff>
--- a/spec/fixtures/Invalid.xlsx
+++ b/spec/fixtures/Invalid.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -29,20 +29,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Last Name</t>
   </si>
   <si>
-    <t>1st name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grade </t>
-  </si>
-  <si>
-    <t>parents preferred email</t>
-  </si>
-  <si>
     <t>Cardinal Gibbons HS Group</t>
   </si>
   <si>
@@ -74,13 +65,34 @@
   </si>
   <si>
     <t>Britney</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Teen Name</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>School</t>
+  </si>
+  <si>
+    <t>Teen Email</t>
+  </si>
+  <si>
+    <t>Parent Email Address(es)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -93,8 +105,14 @@
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -107,8 +125,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -131,6 +155,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
@@ -138,14 +177,14 @@
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1333,106 +1372,140 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="46.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="1" customWidth="1"/>
-    <col min="7" max="256" width="8.83203125" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="7" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="1" customWidth="1"/>
+    <col min="5" max="7" width="8.83203125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="46.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" style="1" customWidth="1"/>
+    <col min="11" max="260" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="J1"/>
+    </row>
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5" t="s">
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="I5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="4"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1451,79 +1524,79 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="8.83203125" style="8" customWidth="1"/>
+    <col min="1" max="5" width="8.83203125" style="6" customWidth="1"/>
     <col min="6" max="256" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1542,79 +1615,79 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="8.83203125" style="9" customWidth="1"/>
+    <col min="1" max="5" width="8.83203125" style="7" customWidth="1"/>
     <col min="6" max="256" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>